<commit_message>
Added new graphic assets of businext project.
</commit_message>
<xml_diff>
--- a/files/system/import-clients-sample.xlsx
+++ b/files/system/import-clients-sample.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D2F73A-D622-4429-A132-5221556C3E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,24 +128,6 @@
     <t>Cox</t>
   </si>
   <si>
-    <t>client1@demo.com</t>
-  </si>
-  <si>
-    <t>client2@demo.com</t>
-  </si>
-  <si>
-    <t>client3@demo.com</t>
-  </si>
-  <si>
-    <t>client4@demo.com</t>
-  </si>
-  <si>
-    <t>client5@demo.com</t>
-  </si>
-  <si>
-    <t>client6@demo.com</t>
-  </si>
-  <si>
     <t>Bradley</t>
   </si>
   <si>
@@ -173,12 +156,30 @@
   </si>
   <si>
     <t>Kelly</t>
+  </si>
+  <si>
+    <t>client1@bytescrafter.net</t>
+  </si>
+  <si>
+    <t>client2@bytescrafter.net</t>
+  </si>
+  <si>
+    <t>client3@bytescrafter.net</t>
+  </si>
+  <si>
+    <t>client4@bytescrafter.net</t>
+  </si>
+  <si>
+    <t>client5@bytescrafter.net</t>
+  </si>
+  <si>
+    <t>client6@bytescrafter.net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,13 +239,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,6 +340,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -373,6 +392,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,8 +666,8 @@
       <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>37</v>
+      <c r="D2" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -672,13 +708,13 @@
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
         <v>38</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>21</v>
@@ -719,13 +755,13 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
@@ -766,13 +802,13 @@
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>21</v>
@@ -813,13 +849,13 @@
         <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
@@ -860,13 +896,13 @@
         <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>21</v>

</xml_diff>